<commit_message>
STILL WORKING ON A SIMPLIFIED MENU DRIVEN PROGRAM. SUCCESSFUL SO FAR!
</commit_message>
<xml_diff>
--- a/Arduino/PROTOTYPE4/MENU_DRIVEN_PROGRAM_FLOWCHART.xlsx
+++ b/Arduino/PROTOTYPE4/MENU_DRIVEN_PROGRAM_FLOWCHART.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Braedin Butler\Google Drive\v^SPEED VARIO PROJECT\DOCUMENTATION\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Braedin Butler\Desktop\vSpeedVario\Arduino\PROTOTYPE4\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -625,22 +625,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -662,6 +653,18 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -990,143 +993,148 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="23"/>
+      <c r="S1" s="23"/>
+      <c r="T1" s="23"/>
+      <c r="U1" s="23"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="3" t="s">
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="24"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="24"/>
+      <c r="P2" s="24"/>
+      <c r="Q2" s="24"/>
+      <c r="R2" s="24"/>
+      <c r="S2" s="24"/>
+      <c r="T2" s="24"/>
+      <c r="U2" s="24"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="3" t="s">
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+      <c r="H3" s="23"/>
+      <c r="I3" s="23"/>
+      <c r="J3" s="23"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
-      <c r="T3" s="3"/>
-      <c r="U3" s="3"/>
+      <c r="M3" s="24"/>
+      <c r="N3" s="24"/>
+      <c r="O3" s="24"/>
+      <c r="P3" s="24"/>
+      <c r="Q3" s="24"/>
+      <c r="R3" s="24"/>
+      <c r="S3" s="24"/>
+      <c r="T3" s="24"/>
+      <c r="U3" s="24"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="3" t="s">
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
-      <c r="R4" s="3"/>
-      <c r="S4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="U4" s="3"/>
+      <c r="O4" s="24"/>
+      <c r="P4" s="24"/>
+      <c r="Q4" s="24"/>
+      <c r="R4" s="24"/>
+      <c r="S4" s="24"/>
+      <c r="T4" s="24"/>
+      <c r="U4" s="24"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="5"/>
-      <c r="K5" s="5"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="2" t="s">
+      <c r="E5" s="23"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="2"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="3"/>
-      <c r="S5" s="3"/>
-      <c r="T5" s="3"/>
-      <c r="U5" s="3"/>
+      <c r="O5" s="23"/>
+      <c r="P5" s="23"/>
+      <c r="Q5" s="23"/>
+      <c r="R5" s="24"/>
+      <c r="S5" s="24"/>
+      <c r="T5" s="24"/>
+      <c r="U5" s="24"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="N6" s="2" t="s">
+      <c r="N6" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="O6" s="2"/>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="3"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
-      <c r="T6" s="3"/>
-      <c r="U6" s="3"/>
+      <c r="O6" s="23"/>
+      <c r="P6" s="24"/>
+      <c r="Q6" s="24"/>
+      <c r="R6" s="23"/>
+      <c r="S6" s="23"/>
+      <c r="T6" s="24"/>
+      <c r="U6" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A1:U1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:U2"/>
+    <mergeCell ref="D3:K3"/>
+    <mergeCell ref="L3:U3"/>
     <mergeCell ref="N6:O6"/>
     <mergeCell ref="P6:Q6"/>
     <mergeCell ref="R6:S6"/>
@@ -1138,11 +1146,6 @@
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="R5:U5"/>
     <mergeCell ref="N5:Q5"/>
-    <mergeCell ref="A1:U1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:U2"/>
-    <mergeCell ref="D3:K3"/>
-    <mergeCell ref="L3:U3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1152,76 +1155,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AQ91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="Y5" sqref="Y5:Y10"/>
+    <sheetView tabSelected="1" topLeftCell="S40" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="AG8" sqref="AG8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.875" style="7" customWidth="1"/>
-    <col min="2" max="2" width="21.125" style="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="2.75" style="18" customWidth="1"/>
-    <col min="4" max="4" width="2.875" style="7" customWidth="1"/>
-    <col min="5" max="5" width="2.5" style="7" customWidth="1"/>
-    <col min="6" max="6" width="16.25" style="7" customWidth="1"/>
-    <col min="7" max="7" width="2.5" style="7" customWidth="1"/>
-    <col min="8" max="8" width="18.5" style="7" customWidth="1"/>
-    <col min="9" max="9" width="6" style="7" customWidth="1"/>
-    <col min="10" max="13" width="2.875" style="7" customWidth="1"/>
-    <col min="14" max="14" width="3.125" style="7" customWidth="1"/>
-    <col min="15" max="15" width="17.75" style="7" customWidth="1"/>
-    <col min="16" max="16" width="12" style="7" bestFit="1" customWidth="1"/>
-    <col min="17" max="22" width="3" style="7" customWidth="1"/>
-    <col min="23" max="23" width="2.5" style="7" customWidth="1"/>
-    <col min="24" max="24" width="2.875" style="7" customWidth="1"/>
-    <col min="25" max="25" width="17.875" style="7" customWidth="1"/>
-    <col min="26" max="26" width="9.75" style="7" customWidth="1"/>
-    <col min="27" max="31" width="3" style="7" customWidth="1"/>
-    <col min="32" max="32" width="2.625" style="7" customWidth="1"/>
-    <col min="33" max="35" width="2.5" style="7" customWidth="1"/>
-    <col min="36" max="36" width="2.75" style="7" customWidth="1"/>
-    <col min="37" max="37" width="2.875" style="7" customWidth="1"/>
-    <col min="38" max="38" width="2.5" style="7" customWidth="1"/>
-    <col min="39" max="39" width="17.875" style="7" customWidth="1"/>
-    <col min="40" max="40" width="13.5" style="7" customWidth="1"/>
-    <col min="41" max="16384" width="9" style="7"/>
+    <col min="1" max="1" width="2.875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="21.125" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.75" style="15" customWidth="1"/>
+    <col min="4" max="4" width="2.875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="2.5" style="4" customWidth="1"/>
+    <col min="6" max="6" width="16.25" style="4" customWidth="1"/>
+    <col min="7" max="7" width="2.5" style="4" customWidth="1"/>
+    <col min="8" max="8" width="18.5" style="4" customWidth="1"/>
+    <col min="9" max="9" width="6" style="4" customWidth="1"/>
+    <col min="10" max="13" width="2.875" style="4" customWidth="1"/>
+    <col min="14" max="14" width="3.125" style="4" customWidth="1"/>
+    <col min="15" max="15" width="17.75" style="4" customWidth="1"/>
+    <col min="16" max="16" width="12" style="4" bestFit="1" customWidth="1"/>
+    <col min="17" max="22" width="3" style="4" customWidth="1"/>
+    <col min="23" max="23" width="2.5" style="4" customWidth="1"/>
+    <col min="24" max="24" width="2.875" style="4" customWidth="1"/>
+    <col min="25" max="25" width="17.875" style="4" customWidth="1"/>
+    <col min="26" max="26" width="9.75" style="4" customWidth="1"/>
+    <col min="27" max="31" width="3" style="4" customWidth="1"/>
+    <col min="32" max="32" width="2.625" style="4" customWidth="1"/>
+    <col min="33" max="35" width="2.5" style="4" customWidth="1"/>
+    <col min="36" max="36" width="2.75" style="4" customWidth="1"/>
+    <col min="37" max="37" width="2.875" style="4" customWidth="1"/>
+    <col min="38" max="38" width="2.5" style="4" customWidth="1"/>
+    <col min="39" max="39" width="17.875" style="4" customWidth="1"/>
+    <col min="40" max="40" width="13.5" style="4" customWidth="1"/>
+    <col min="41" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="AQ1" s="7" t="s">
+      <c r="AQ1" s="4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="G2"/>
-      <c r="H2"/>
-      <c r="I2"/>
-      <c r="J2"/>
-      <c r="K2"/>
-      <c r="L2"/>
-      <c r="M2"/>
-      <c r="N2"/>
-      <c r="O2"/>
-      <c r="P2"/>
-      <c r="Q2"/>
-      <c r="R2"/>
-      <c r="S2"/>
-      <c r="T2"/>
-      <c r="U2"/>
-      <c r="V2"/>
-      <c r="W2"/>
-      <c r="X2"/>
-      <c r="Y2"/>
-      <c r="Z2"/>
-      <c r="AA2"/>
-      <c r="AB2"/>
-      <c r="AC2"/>
-      <c r="AD2"/>
-      <c r="AE2"/>
-      <c r="AF2"/>
-    </row>
+    <row r="2" spans="2:43" s="26" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="15" t="s">
         <v>86</v>
       </c>
       <c r="E3"/>
@@ -1254,7 +1230,7 @@
       <c r="AF3"/>
     </row>
     <row r="4" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="15" t="s">
         <v>91</v>
       </c>
       <c r="E4"/>
@@ -1295,30 +1271,30 @@
       <c r="AF4"/>
     </row>
     <row r="5" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="16" t="s">
         <v>90</v>
       </c>
       <c r="D5"/>
       <c r="E5"/>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="25" t="s">
         <v>155</v>
       </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="8" t="s">
+      <c r="G5" s="6"/>
+      <c r="H5" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="14" t="s">
+      <c r="I5" s="11" t="s">
         <v>23</v>
       </c>
       <c r="J5"/>
       <c r="K5"/>
       <c r="L5"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10"/>
-      <c r="O5" s="8" t="s">
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="P5" s="9" t="s">
+      <c r="P5" s="6" t="s">
         <v>88</v>
       </c>
       <c r="Q5"/>
@@ -1326,12 +1302,12 @@
       <c r="S5"/>
       <c r="T5"/>
       <c r="U5"/>
-      <c r="W5" s="10"/>
-      <c r="X5" s="10"/>
-      <c r="Y5" s="8" t="s">
+      <c r="W5" s="7"/>
+      <c r="X5" s="7"/>
+      <c r="Y5" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="Z5" s="9" t="s">
+      <c r="Z5" s="6" t="s">
         <v>24</v>
       </c>
       <c r="AA5"/>
@@ -1345,37 +1321,37 @@
       <c r="AI5"/>
     </row>
     <row r="6" spans="2:43" x14ac:dyDescent="0.25">
-      <c r="B6" s="18" t="s">
+      <c r="B6" s="15" t="s">
         <v>87</v>
       </c>
       <c r="D6"/>
       <c r="E6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="8" t="s">
+      <c r="F6" s="25"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="I6" s="21" t="s">
+      <c r="I6" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="O6" s="8" t="s">
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="O6" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="P6" s="21" t="s">
+      <c r="P6" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="Q6" s="10"/>
-      <c r="R6" s="10"/>
-      <c r="S6" s="10"/>
-      <c r="T6" s="10"/>
-      <c r="U6" s="10"/>
-      <c r="V6" s="10"/>
-      <c r="W6" s="10"/>
-      <c r="Y6" s="8" t="s">
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="7"/>
+      <c r="U6" s="7"/>
+      <c r="V6" s="7"/>
+      <c r="W6" s="7"/>
+      <c r="Y6" s="5" t="s">
         <v>59</v>
       </c>
       <c r="Z6" t="s">
@@ -1388,32 +1364,32 @@
     <row r="7" spans="2:43" x14ac:dyDescent="0.25">
       <c r="D7"/>
       <c r="E7"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="8" t="s">
+      <c r="F7" s="25"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="I7" s="22" t="s">
+      <c r="I7" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11"/>
-      <c r="M7" s="11"/>
-      <c r="O7" s="8" t="s">
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="O7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="P7" s="22" t="s">
+      <c r="P7" s="19" t="s">
         <v>156</v>
       </c>
-      <c r="Q7" s="11"/>
-      <c r="R7" s="11"/>
-      <c r="S7" s="11"/>
-      <c r="T7" s="11"/>
-      <c r="U7" s="11"/>
-      <c r="V7" s="11"/>
-      <c r="W7" s="11"/>
-      <c r="Y7" s="8" t="s">
+      <c r="Q7" s="8"/>
+      <c r="R7" s="8"/>
+      <c r="S7" s="8"/>
+      <c r="T7" s="8"/>
+      <c r="U7" s="8"/>
+      <c r="V7" s="8"/>
+      <c r="W7" s="8"/>
+      <c r="Y7" s="5" t="s">
         <v>30</v>
       </c>
       <c r="Z7" t="s">
@@ -1426,32 +1402,32 @@
     <row r="8" spans="2:43" x14ac:dyDescent="0.25">
       <c r="D8"/>
       <c r="E8"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="8" t="s">
+      <c r="F8" s="25"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="I8" s="23" t="s">
+      <c r="I8" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="J8" s="12"/>
-      <c r="K8" s="12"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="11"/>
-      <c r="O8" s="8" t="s">
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="8"/>
+      <c r="O8" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="P8" s="23" t="s">
+      <c r="P8" s="20" t="s">
         <v>157</v>
       </c>
-      <c r="Q8" s="12"/>
-      <c r="R8" s="12"/>
-      <c r="S8" s="12"/>
-      <c r="T8" s="12"/>
-      <c r="U8" s="12"/>
-      <c r="V8" s="12"/>
-      <c r="W8" s="11"/>
-      <c r="Y8" s="8" t="s">
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9"/>
+      <c r="S8" s="9"/>
+      <c r="T8" s="9"/>
+      <c r="U8" s="9"/>
+      <c r="V8" s="9"/>
+      <c r="W8" s="8"/>
+      <c r="Y8" s="5" t="s">
         <v>16</v>
       </c>
       <c r="Z8" t="s">
@@ -1464,22 +1440,22 @@
     <row r="9" spans="2:43" x14ac:dyDescent="0.25">
       <c r="D9"/>
       <c r="E9"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="8" t="s">
+      <c r="F9" s="25"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="I9" s="24" t="s">
+      <c r="I9" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="11"/>
-      <c r="O9" s="8"/>
-      <c r="V9" s="12"/>
-      <c r="W9" s="11"/>
-      <c r="Y9" s="16" t="s">
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="8"/>
+      <c r="O9" s="5"/>
+      <c r="V9" s="9"/>
+      <c r="W9" s="8"/>
+      <c r="Y9" s="13" t="s">
         <v>38</v>
       </c>
       <c r="Z9" t="s">
@@ -1492,34 +1468,34 @@
     <row r="10" spans="2:43" x14ac:dyDescent="0.25">
       <c r="D10"/>
       <c r="E10"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="8" t="s">
+      <c r="F10" s="25"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I10" s="14" t="s">
+      <c r="I10" s="11" t="s">
         <v>23</v>
       </c>
       <c r="J10"/>
-      <c r="K10" s="13"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="11"/>
-      <c r="O10" s="8" t="s">
+      <c r="K10" s="10"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="8"/>
+      <c r="O10" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="P10" s="14" t="s">
+      <c r="P10" s="11" t="s">
         <v>23</v>
       </c>
       <c r="Q10"/>
       <c r="R10"/>
       <c r="S10"/>
       <c r="T10"/>
-      <c r="V10" s="12"/>
-      <c r="W10" s="11"/>
-      <c r="Y10" s="8" t="s">
+      <c r="V10" s="9"/>
+      <c r="W10" s="8"/>
+      <c r="Y10" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="Z10" s="14" t="s">
+      <c r="Z10" s="11" t="s">
         <v>23</v>
       </c>
       <c r="AA10"/>
@@ -1540,9 +1516,9 @@
       <c r="H11"/>
       <c r="I11"/>
       <c r="J11"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="11"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="8"/>
       <c r="N11"/>
       <c r="O11"/>
       <c r="P11"/>
@@ -1550,8 +1526,8 @@
       <c r="R11"/>
       <c r="S11"/>
       <c r="T11"/>
-      <c r="V11" s="12"/>
-      <c r="W11" s="11"/>
+      <c r="V11" s="9"/>
+      <c r="W11" s="8"/>
       <c r="X11"/>
       <c r="Y11"/>
       <c r="Z11"/>
@@ -1573,9 +1549,9 @@
       <c r="H12"/>
       <c r="I12"/>
       <c r="J12"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="11"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="8"/>
       <c r="N12"/>
       <c r="O12"/>
       <c r="P12"/>
@@ -1583,8 +1559,8 @@
       <c r="R12"/>
       <c r="S12"/>
       <c r="T12"/>
-      <c r="V12" s="12"/>
-      <c r="W12" s="11"/>
+      <c r="V12" s="9"/>
+      <c r="W12" s="8"/>
       <c r="X12"/>
       <c r="Y12"/>
       <c r="Z12"/>
@@ -1606,23 +1582,23 @@
       <c r="H13"/>
       <c r="I13"/>
       <c r="J13"/>
-      <c r="K13" s="13"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="11"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="8"/>
       <c r="N13"/>
       <c r="O13" s="1">
         <v>12</v>
       </c>
       <c r="P13"/>
-      <c r="V13" s="12"/>
-      <c r="W13" s="11"/>
-      <c r="Y13" s="20">
+      <c r="V13" s="9"/>
+      <c r="W13" s="8"/>
+      <c r="Y13" s="17">
         <v>4</v>
       </c>
       <c r="AG13"/>
       <c r="AH13"/>
       <c r="AI13"/>
-      <c r="AM13" s="20">
+      <c r="AM13" s="17">
         <v>5</v>
       </c>
     </row>
@@ -1630,27 +1606,27 @@
       <c r="D14"/>
       <c r="E14"/>
       <c r="I14"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="11"/>
-      <c r="N14" s="11"/>
-      <c r="O14" s="8" t="s">
+      <c r="K14" s="14"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="P14" s="9" t="s">
+      <c r="P14" s="6" t="s">
         <v>88</v>
       </c>
       <c r="Q14"/>
       <c r="R14"/>
       <c r="S14"/>
       <c r="T14"/>
-      <c r="V14" s="12"/>
-      <c r="W14" s="11"/>
-      <c r="X14" s="11"/>
-      <c r="Y14" s="8" t="s">
+      <c r="V14" s="9"/>
+      <c r="W14" s="8"/>
+      <c r="X14" s="8"/>
+      <c r="Y14" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="Z14" s="9" t="s">
+      <c r="Z14" s="6" t="s">
         <v>24</v>
       </c>
       <c r="AA14"/>
@@ -1662,12 +1638,12 @@
       <c r="AG14"/>
       <c r="AH14"/>
       <c r="AI14"/>
-      <c r="AK14" s="10"/>
-      <c r="AL14" s="10"/>
-      <c r="AM14" s="8" t="s">
+      <c r="AK14" s="7"/>
+      <c r="AL14" s="7"/>
+      <c r="AM14" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="AN14" s="9" t="s">
+      <c r="AN14" s="6" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1675,9 +1651,9 @@
       <c r="D15"/>
       <c r="E15"/>
       <c r="I15"/>
-      <c r="K15" s="17"/>
-      <c r="L15" s="12"/>
-      <c r="O15" s="16" t="s">
+      <c r="K15" s="14"/>
+      <c r="L15" s="9"/>
+      <c r="O15" s="13" t="s">
         <v>56</v>
       </c>
       <c r="P15" t="s">
@@ -1687,25 +1663,25 @@
       <c r="R15"/>
       <c r="S15"/>
       <c r="T15"/>
-      <c r="V15" s="12"/>
-      <c r="Y15" s="8" t="s">
+      <c r="V15" s="9"/>
+      <c r="Y15" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="Z15" s="25" t="s">
+      <c r="Z15" s="22" t="s">
         <v>160</v>
       </c>
-      <c r="AA15" s="10"/>
-      <c r="AB15" s="10"/>
-      <c r="AC15" s="10"/>
-      <c r="AD15" s="10"/>
-      <c r="AE15" s="10"/>
-      <c r="AF15" s="10"/>
-      <c r="AG15" s="10"/>
-      <c r="AH15" s="10"/>
-      <c r="AI15" s="10"/>
-      <c r="AJ15" s="10"/>
-      <c r="AK15" s="10"/>
-      <c r="AM15" s="8" t="s">
+      <c r="AA15" s="7"/>
+      <c r="AB15" s="7"/>
+      <c r="AC15" s="7"/>
+      <c r="AD15" s="7"/>
+      <c r="AE15" s="7"/>
+      <c r="AF15" s="7"/>
+      <c r="AG15" s="7"/>
+      <c r="AH15" s="7"/>
+      <c r="AI15" s="7"/>
+      <c r="AJ15" s="7"/>
+      <c r="AK15" s="7"/>
+      <c r="AM15" s="5" t="s">
         <v>67</v>
       </c>
       <c r="AN15" t="s">
@@ -1716,33 +1692,33 @@
       <c r="D16"/>
       <c r="E16"/>
       <c r="I16"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="12"/>
-      <c r="O16" s="8" t="s">
+      <c r="K16" s="14"/>
+      <c r="L16" s="9"/>
+      <c r="O16" s="5" t="s">
         <v>27</v>
       </c>
       <c r="P16" t="s">
         <v>29</v>
       </c>
-      <c r="V16" s="12"/>
-      <c r="Y16" s="8" t="s">
+      <c r="V16" s="9"/>
+      <c r="Y16" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="Z16" s="22" t="s">
+      <c r="Z16" s="19" t="s">
         <v>161</v>
       </c>
-      <c r="AA16" s="11"/>
-      <c r="AB16" s="11"/>
-      <c r="AC16" s="11"/>
-      <c r="AD16" s="11"/>
-      <c r="AE16" s="11"/>
-      <c r="AF16" s="11"/>
-      <c r="AG16" s="11"/>
-      <c r="AH16" s="11"/>
-      <c r="AI16" s="11"/>
-      <c r="AJ16" s="11"/>
-      <c r="AK16" s="11"/>
-      <c r="AM16" s="8" t="s">
+      <c r="AA16" s="8"/>
+      <c r="AB16" s="8"/>
+      <c r="AC16" s="8"/>
+      <c r="AD16" s="8"/>
+      <c r="AE16" s="8"/>
+      <c r="AF16" s="8"/>
+      <c r="AG16" s="8"/>
+      <c r="AH16" s="8"/>
+      <c r="AI16" s="8"/>
+      <c r="AJ16" s="8"/>
+      <c r="AK16" s="8"/>
+      <c r="AM16" s="5" t="s">
         <v>33</v>
       </c>
       <c r="AN16" t="s">
@@ -1753,59 +1729,59 @@
       <c r="D17"/>
       <c r="E17"/>
       <c r="I17"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="12"/>
-      <c r="O17" s="16" t="s">
+      <c r="K17" s="14"/>
+      <c r="L17" s="9"/>
+      <c r="O17" s="13" t="s">
         <v>37</v>
       </c>
       <c r="P17" t="s">
         <v>29</v>
       </c>
-      <c r="V17" s="12"/>
-      <c r="Y17" s="8"/>
-      <c r="AK17" s="11"/>
-      <c r="AM17" s="8"/>
+      <c r="V17" s="9"/>
+      <c r="Y17" s="5"/>
+      <c r="AK17" s="8"/>
+      <c r="AM17" s="5"/>
       <c r="AN17"/>
     </row>
     <row r="18" spans="4:40" x14ac:dyDescent="0.25">
       <c r="D18"/>
       <c r="E18"/>
       <c r="I18"/>
-      <c r="K18" s="17"/>
-      <c r="L18" s="12"/>
-      <c r="O18" s="8" t="s">
+      <c r="K18" s="14"/>
+      <c r="L18" s="9"/>
+      <c r="O18" s="5" t="s">
         <v>28</v>
       </c>
       <c r="P18" t="s">
         <v>29</v>
       </c>
-      <c r="V18" s="12"/>
-      <c r="Y18" s="8"/>
-      <c r="AK18" s="11"/>
-      <c r="AM18" s="8"/>
+      <c r="V18" s="9"/>
+      <c r="Y18" s="5"/>
+      <c r="AK18" s="8"/>
+      <c r="AM18" s="5"/>
       <c r="AN18"/>
     </row>
     <row r="19" spans="4:40" x14ac:dyDescent="0.25">
       <c r="D19"/>
       <c r="E19"/>
       <c r="I19"/>
-      <c r="K19" s="17"/>
-      <c r="L19" s="12"/>
-      <c r="O19" s="8" t="s">
+      <c r="K19" s="14"/>
+      <c r="L19" s="9"/>
+      <c r="O19" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="P19" s="14" t="s">
+      <c r="P19" s="11" t="s">
         <v>23</v>
       </c>
       <c r="Q19"/>
       <c r="R19"/>
       <c r="S19"/>
       <c r="T19"/>
-      <c r="V19" s="12"/>
-      <c r="Y19" s="8" t="s">
+      <c r="V19" s="9"/>
+      <c r="Y19" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="Z19" s="14" t="s">
+      <c r="Z19" s="11" t="s">
         <v>23</v>
       </c>
       <c r="AA19"/>
@@ -1814,19 +1790,19 @@
       <c r="AD19"/>
       <c r="AE19"/>
       <c r="AF19"/>
-      <c r="AK19" s="11"/>
-      <c r="AM19" s="8" t="s">
+      <c r="AK19" s="8"/>
+      <c r="AM19" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="AN19" s="14" t="s">
+      <c r="AN19" s="11" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="20" spans="4:40" x14ac:dyDescent="0.25">
       <c r="D20"/>
       <c r="E20"/>
-      <c r="K20" s="17"/>
-      <c r="L20" s="12"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="9"/>
       <c r="M20"/>
       <c r="N20"/>
       <c r="O20"/>
@@ -1835,7 +1811,7 @@
       <c r="R20"/>
       <c r="S20"/>
       <c r="T20"/>
-      <c r="V20" s="12"/>
+      <c r="V20" s="9"/>
       <c r="W20"/>
       <c r="X20"/>
       <c r="Y20"/>
@@ -1846,7 +1822,7 @@
       <c r="AD20"/>
       <c r="AE20"/>
       <c r="AF20"/>
-      <c r="AK20" s="11"/>
+      <c r="AK20" s="8"/>
     </row>
     <row r="21" spans="4:40" x14ac:dyDescent="0.25">
       <c r="D21"/>
@@ -1856,8 +1832,8 @@
       <c r="H21"/>
       <c r="I21"/>
       <c r="J21"/>
-      <c r="K21" s="17"/>
-      <c r="L21" s="12"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="9"/>
       <c r="M21"/>
       <c r="N21"/>
       <c r="O21"/>
@@ -1866,7 +1842,7 @@
       <c r="R21"/>
       <c r="S21"/>
       <c r="T21"/>
-      <c r="V21" s="12"/>
+      <c r="V21" s="9"/>
       <c r="W21"/>
       <c r="X21"/>
       <c r="Y21"/>
@@ -1877,49 +1853,49 @@
       <c r="AD21"/>
       <c r="AE21"/>
       <c r="AF21"/>
-      <c r="AK21" s="11"/>
+      <c r="AK21" s="8"/>
     </row>
     <row r="22" spans="4:40" x14ac:dyDescent="0.25">
       <c r="D22"/>
       <c r="E22"/>
-      <c r="K22" s="17"/>
-      <c r="L22" s="12"/>
-      <c r="O22" s="20">
+      <c r="K22" s="14"/>
+      <c r="L22" s="9"/>
+      <c r="O22" s="17">
         <v>13</v>
       </c>
-      <c r="V22" s="12"/>
-      <c r="Y22" s="20">
+      <c r="V22" s="9"/>
+      <c r="Y22" s="17">
         <v>7</v>
       </c>
-      <c r="AK22" s="11"/>
-      <c r="AM22" s="20">
+      <c r="AK22" s="8"/>
+      <c r="AM22" s="17">
         <v>6</v>
       </c>
     </row>
     <row r="23" spans="4:40" x14ac:dyDescent="0.25">
       <c r="D23"/>
       <c r="E23"/>
-      <c r="K23" s="17"/>
-      <c r="L23" s="12"/>
-      <c r="M23" s="12"/>
-      <c r="N23" s="12"/>
-      <c r="O23" s="8" t="s">
+      <c r="K23" s="14"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="P23" s="9" t="s">
+      <c r="P23" s="6" t="s">
         <v>88</v>
       </c>
       <c r="Q23"/>
       <c r="R23"/>
       <c r="S23"/>
       <c r="T23"/>
-      <c r="V23" s="12"/>
-      <c r="W23" s="12"/>
-      <c r="X23" s="12"/>
-      <c r="Y23" s="8" t="s">
+      <c r="V23" s="9"/>
+      <c r="W23" s="9"/>
+      <c r="X23" s="9"/>
+      <c r="Y23" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="Z23" s="9" t="s">
+      <c r="Z23" s="6" t="s">
         <v>24</v>
       </c>
       <c r="AA23"/>
@@ -1931,45 +1907,45 @@
       <c r="AG23"/>
       <c r="AH23"/>
       <c r="AI23"/>
-      <c r="AK23" s="11"/>
-      <c r="AL23" s="11"/>
-      <c r="AM23" s="8" t="s">
+      <c r="AK23" s="8"/>
+      <c r="AL23" s="8"/>
+      <c r="AM23" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="AN23" s="9" t="s">
+      <c r="AN23" s="6" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="24" spans="4:40" x14ac:dyDescent="0.25">
       <c r="D24"/>
       <c r="E24"/>
-      <c r="K24" s="17"/>
-      <c r="O24" s="8" t="s">
+      <c r="K24" s="14"/>
+      <c r="O24" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="P24" s="21" t="s">
+      <c r="P24" s="18" t="s">
         <v>158</v>
       </c>
-      <c r="Q24" s="10"/>
-      <c r="R24" s="10"/>
-      <c r="S24" s="10"/>
-      <c r="T24" s="10"/>
-      <c r="Y24" s="8" t="s">
+      <c r="Q24" s="7"/>
+      <c r="R24" s="7"/>
+      <c r="S24" s="7"/>
+      <c r="T24" s="7"/>
+      <c r="Y24" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="Z24" s="21" t="s">
+      <c r="Z24" s="18" t="s">
         <v>162</v>
       </c>
-      <c r="AA24" s="10"/>
-      <c r="AB24" s="10"/>
-      <c r="AC24" s="10"/>
-      <c r="AD24" s="10"/>
-      <c r="AE24" s="10"/>
-      <c r="AF24" s="10"/>
-      <c r="AG24" s="10"/>
-      <c r="AH24" s="10"/>
-      <c r="AI24" s="10"/>
-      <c r="AM24" s="8" t="s">
+      <c r="AA24" s="7"/>
+      <c r="AB24" s="7"/>
+      <c r="AC24" s="7"/>
+      <c r="AD24" s="7"/>
+      <c r="AE24" s="7"/>
+      <c r="AF24" s="7"/>
+      <c r="AG24" s="7"/>
+      <c r="AH24" s="7"/>
+      <c r="AI24" s="7"/>
+      <c r="AM24" s="5" t="s">
         <v>68</v>
       </c>
       <c r="AN24" t="s">
@@ -1979,30 +1955,30 @@
     <row r="25" spans="4:40" x14ac:dyDescent="0.25">
       <c r="D25"/>
       <c r="E25"/>
-      <c r="K25" s="17"/>
-      <c r="O25" s="16" t="s">
+      <c r="K25" s="14"/>
+      <c r="O25" s="13" t="s">
         <v>37</v>
       </c>
       <c r="P25" t="s">
         <v>29</v>
       </c>
-      <c r="T25" s="5"/>
-      <c r="Y25" s="8" t="s">
+      <c r="T25" s="3"/>
+      <c r="Y25" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="Z25" s="22" t="s">
+      <c r="Z25" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="AA25" s="11"/>
-      <c r="AB25" s="11"/>
-      <c r="AC25" s="11"/>
-      <c r="AD25" s="11"/>
-      <c r="AE25" s="11"/>
-      <c r="AF25" s="11"/>
-      <c r="AG25" s="11"/>
-      <c r="AH25" s="11"/>
-      <c r="AI25" s="10"/>
-      <c r="AM25" s="8" t="s">
+      <c r="AA25" s="8"/>
+      <c r="AB25" s="8"/>
+      <c r="AC25" s="8"/>
+      <c r="AD25" s="8"/>
+      <c r="AE25" s="8"/>
+      <c r="AF25" s="8"/>
+      <c r="AG25" s="8"/>
+      <c r="AH25" s="8"/>
+      <c r="AI25" s="7"/>
+      <c r="AM25" s="5" t="s">
         <v>32</v>
       </c>
       <c r="AN25" t="s">
@@ -2012,72 +1988,72 @@
     <row r="26" spans="4:40" x14ac:dyDescent="0.25">
       <c r="D26"/>
       <c r="E26"/>
-      <c r="K26" s="17"/>
-      <c r="O26" s="8" t="s">
+      <c r="K26" s="14"/>
+      <c r="O26" s="5" t="s">
         <v>28</v>
       </c>
       <c r="P26" t="s">
         <v>29</v>
       </c>
-      <c r="T26" s="10"/>
-      <c r="Y26" s="8" t="s">
+      <c r="T26" s="7"/>
+      <c r="Y26" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="Z26" s="23" t="s">
+      <c r="Z26" s="20" t="s">
         <v>164</v>
       </c>
-      <c r="AA26" s="12"/>
-      <c r="AB26" s="12"/>
-      <c r="AC26" s="12"/>
-      <c r="AD26" s="12"/>
-      <c r="AE26" s="12"/>
-      <c r="AF26" s="12"/>
-      <c r="AG26" s="12"/>
-      <c r="AH26" s="11"/>
-      <c r="AI26" s="10"/>
-      <c r="AM26" s="8"/>
+      <c r="AA26" s="9"/>
+      <c r="AB26" s="9"/>
+      <c r="AC26" s="9"/>
+      <c r="AD26" s="9"/>
+      <c r="AE26" s="9"/>
+      <c r="AF26" s="9"/>
+      <c r="AG26" s="9"/>
+      <c r="AH26" s="8"/>
+      <c r="AI26" s="7"/>
+      <c r="AM26" s="5"/>
       <c r="AN26"/>
     </row>
     <row r="27" spans="4:40" x14ac:dyDescent="0.25">
       <c r="D27"/>
       <c r="E27"/>
-      <c r="K27" s="17"/>
-      <c r="O27" s="8"/>
-      <c r="T27" s="10"/>
-      <c r="Y27" s="8" t="s">
+      <c r="K27" s="14"/>
+      <c r="O27" s="5"/>
+      <c r="T27" s="7"/>
+      <c r="Y27" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="Z27" s="24" t="s">
+      <c r="Z27" s="21" t="s">
         <v>165</v>
       </c>
-      <c r="AA27" s="13"/>
-      <c r="AB27" s="13"/>
-      <c r="AC27" s="13"/>
-      <c r="AD27" s="13"/>
-      <c r="AE27" s="13"/>
-      <c r="AF27" s="13"/>
-      <c r="AG27" s="12"/>
-      <c r="AH27" s="11"/>
-      <c r="AI27" s="10"/>
-      <c r="AM27" s="8"/>
+      <c r="AA27" s="10"/>
+      <c r="AB27" s="10"/>
+      <c r="AC27" s="10"/>
+      <c r="AD27" s="10"/>
+      <c r="AE27" s="10"/>
+      <c r="AF27" s="10"/>
+      <c r="AG27" s="9"/>
+      <c r="AH27" s="8"/>
+      <c r="AI27" s="7"/>
+      <c r="AM27" s="5"/>
       <c r="AN27"/>
     </row>
     <row r="28" spans="4:40" x14ac:dyDescent="0.25">
       <c r="D28"/>
       <c r="E28"/>
-      <c r="K28" s="17"/>
-      <c r="O28" s="8" t="s">
+      <c r="K28" s="14"/>
+      <c r="O28" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="P28" s="14" t="s">
+      <c r="P28" s="11" t="s">
         <v>23</v>
       </c>
       <c r="Q28"/>
-      <c r="T28" s="10"/>
-      <c r="Y28" s="8" t="s">
+      <c r="T28" s="7"/>
+      <c r="Y28" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="Z28" s="14" t="s">
+      <c r="Z28" s="11" t="s">
         <v>23</v>
       </c>
       <c r="AA28"/>
@@ -2085,14 +2061,14 @@
       <c r="AC28"/>
       <c r="AD28"/>
       <c r="AE28"/>
-      <c r="AF28" s="17"/>
-      <c r="AG28" s="12"/>
-      <c r="AH28" s="11"/>
-      <c r="AI28" s="10"/>
-      <c r="AM28" s="8" t="s">
+      <c r="AF28" s="14"/>
+      <c r="AG28" s="9"/>
+      <c r="AH28" s="8"/>
+      <c r="AI28" s="7"/>
+      <c r="AM28" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="AN28" s="14" t="s">
+      <c r="AN28" s="11" t="s">
         <v>23</v>
       </c>
     </row>
@@ -2104,18 +2080,18 @@
       <c r="H29"/>
       <c r="I29"/>
       <c r="J29"/>
-      <c r="K29" s="17"/>
+      <c r="K29" s="14"/>
       <c r="L29"/>
       <c r="M29"/>
       <c r="N29"/>
       <c r="O29"/>
       <c r="P29"/>
       <c r="Q29"/>
-      <c r="T29" s="5"/>
-      <c r="AF29" s="13"/>
-      <c r="AG29" s="12"/>
-      <c r="AH29" s="11"/>
-      <c r="AI29" s="10"/>
+      <c r="T29" s="3"/>
+      <c r="AF29" s="10"/>
+      <c r="AG29" s="9"/>
+      <c r="AH29" s="8"/>
+      <c r="AI29" s="7"/>
     </row>
     <row r="30" spans="4:40" x14ac:dyDescent="0.25">
       <c r="D30"/>
@@ -2125,95 +2101,95 @@
       <c r="H30"/>
       <c r="I30"/>
       <c r="J30"/>
-      <c r="K30" s="17"/>
+      <c r="K30" s="14"/>
       <c r="L30"/>
       <c r="M30"/>
       <c r="N30"/>
       <c r="O30"/>
       <c r="P30"/>
       <c r="Q30"/>
-      <c r="T30" s="5"/>
+      <c r="T30" s="3"/>
       <c r="V30"/>
       <c r="W30"/>
       <c r="X30"/>
-      <c r="AF30" s="13"/>
-      <c r="AG30" s="12"/>
-      <c r="AH30" s="11"/>
-      <c r="AI30" s="10"/>
+      <c r="AF30" s="10"/>
+      <c r="AG30" s="9"/>
+      <c r="AH30" s="8"/>
+      <c r="AI30" s="7"/>
     </row>
     <row r="31" spans="4:40" x14ac:dyDescent="0.25">
-      <c r="K31" s="13"/>
-      <c r="O31" s="20">
+      <c r="K31" s="10"/>
+      <c r="O31" s="17">
         <v>15</v>
       </c>
-      <c r="T31" s="10"/>
-      <c r="Y31" s="20">
+      <c r="T31" s="7"/>
+      <c r="Y31" s="17">
         <v>14</v>
       </c>
-      <c r="AF31" s="13"/>
-      <c r="AG31" s="12"/>
-      <c r="AH31" s="11"/>
-      <c r="AI31" s="10"/>
-      <c r="AM31" s="20">
+      <c r="AF31" s="10"/>
+      <c r="AG31" s="9"/>
+      <c r="AH31" s="8"/>
+      <c r="AI31" s="7"/>
+      <c r="AM31" s="17">
         <v>8</v>
       </c>
     </row>
     <row r="32" spans="4:40" x14ac:dyDescent="0.25">
-      <c r="K32" s="13"/>
-      <c r="L32" s="13"/>
-      <c r="M32" s="13"/>
-      <c r="N32" s="13"/>
-      <c r="O32" s="8" t="s">
+      <c r="K32" s="10"/>
+      <c r="L32" s="10"/>
+      <c r="M32" s="10"/>
+      <c r="N32" s="10"/>
+      <c r="O32" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="P32" s="9" t="s">
+      <c r="P32" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="T32" s="10"/>
-      <c r="U32" s="10"/>
-      <c r="V32" s="10"/>
-      <c r="W32" s="10"/>
-      <c r="X32" s="10"/>
-      <c r="Y32" s="8" t="s">
+      <c r="T32" s="7"/>
+      <c r="U32" s="7"/>
+      <c r="V32" s="7"/>
+      <c r="W32" s="7"/>
+      <c r="X32" s="7"/>
+      <c r="Y32" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="Z32" s="9" t="s">
+      <c r="Z32" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="AF32" s="13"/>
-      <c r="AG32" s="12"/>
-      <c r="AH32" s="11"/>
-      <c r="AI32" s="10"/>
-      <c r="AJ32" s="10"/>
-      <c r="AK32" s="10"/>
-      <c r="AL32" s="10"/>
-      <c r="AM32" s="8" t="s">
+      <c r="AF32" s="10"/>
+      <c r="AG32" s="9"/>
+      <c r="AH32" s="8"/>
+      <c r="AI32" s="7"/>
+      <c r="AJ32" s="7"/>
+      <c r="AK32" s="7"/>
+      <c r="AL32" s="7"/>
+      <c r="AM32" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="AN32" s="9" t="s">
+      <c r="AN32" s="6" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="33" spans="15:40" x14ac:dyDescent="0.25">
-      <c r="O33" s="8" t="s">
+      <c r="O33" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="P33" s="21" t="s">
+      <c r="P33" s="18" t="s">
         <v>159</v>
       </c>
-      <c r="Q33" s="10"/>
-      <c r="R33" s="10"/>
+      <c r="Q33" s="7"/>
+      <c r="R33" s="7"/>
       <c r="S33"/>
-      <c r="Y33" s="8" t="s">
+      <c r="Y33" s="5" t="s">
         <v>65</v>
       </c>
       <c r="Z33" t="s">
         <v>29</v>
       </c>
-      <c r="AF33" s="13"/>
-      <c r="AG33" s="12"/>
-      <c r="AH33" s="11"/>
-      <c r="AM33" s="8" t="s">
+      <c r="AF33" s="10"/>
+      <c r="AG33" s="9"/>
+      <c r="AH33" s="8"/>
+      <c r="AM33" s="5" t="s">
         <v>69</v>
       </c>
       <c r="AN33" t="s">
@@ -2221,24 +2197,24 @@
       </c>
     </row>
     <row r="34" spans="15:40" x14ac:dyDescent="0.25">
-      <c r="O34" s="16" t="s">
+      <c r="O34" s="13" t="s">
         <v>50</v>
       </c>
       <c r="P34" t="s">
         <v>29</v>
       </c>
-      <c r="R34" s="10"/>
+      <c r="R34" s="7"/>
       <c r="S34"/>
-      <c r="Y34" s="8" t="s">
+      <c r="Y34" s="5" t="s">
         <v>40</v>
       </c>
       <c r="Z34" t="s">
         <v>29</v>
       </c>
-      <c r="AF34" s="13"/>
-      <c r="AG34" s="12"/>
-      <c r="AH34" s="11"/>
-      <c r="AM34" s="8" t="s">
+      <c r="AF34" s="10"/>
+      <c r="AG34" s="9"/>
+      <c r="AH34" s="8"/>
+      <c r="AM34" s="5" t="s">
         <v>42</v>
       </c>
       <c r="AN34" t="s">
@@ -2246,20 +2222,20 @@
       </c>
     </row>
     <row r="35" spans="15:40" x14ac:dyDescent="0.25">
-      <c r="O35" s="8" t="s">
+      <c r="O35" s="5" t="s">
         <v>51</v>
       </c>
       <c r="P35" t="s">
         <v>29</v>
       </c>
-      <c r="R35" s="10"/>
+      <c r="R35" s="7"/>
       <c r="S35"/>
-      <c r="Y35" s="8"/>
+      <c r="Y35" s="5"/>
       <c r="Z35"/>
-      <c r="AF35" s="13"/>
-      <c r="AG35" s="12"/>
-      <c r="AH35" s="11"/>
-      <c r="AM35" s="8" t="s">
+      <c r="AF35" s="10"/>
+      <c r="AG35" s="9"/>
+      <c r="AH35" s="8"/>
+      <c r="AM35" s="5" t="s">
         <v>43</v>
       </c>
       <c r="AN35" t="s">
@@ -2267,20 +2243,20 @@
       </c>
     </row>
     <row r="36" spans="15:40" x14ac:dyDescent="0.25">
-      <c r="O36" s="8" t="s">
+      <c r="O36" s="5" t="s">
         <v>76</v>
       </c>
       <c r="P36" t="s">
         <v>29</v>
       </c>
-      <c r="R36" s="10"/>
+      <c r="R36" s="7"/>
       <c r="S36"/>
-      <c r="Y36" s="8"/>
+      <c r="Y36" s="5"/>
       <c r="Z36"/>
-      <c r="AF36" s="13"/>
-      <c r="AG36" s="12"/>
-      <c r="AH36" s="11"/>
-      <c r="AM36" s="8" t="s">
+      <c r="AF36" s="10"/>
+      <c r="AG36" s="9"/>
+      <c r="AH36" s="8"/>
+      <c r="AM36" s="5" t="s">
         <v>45</v>
       </c>
       <c r="AN36" t="s">
@@ -2288,105 +2264,105 @@
       </c>
     </row>
     <row r="37" spans="15:40" x14ac:dyDescent="0.25">
-      <c r="O37" s="8" t="s">
+      <c r="O37" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="P37" s="14" t="s">
+      <c r="P37" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="R37" s="10"/>
+      <c r="R37" s="7"/>
       <c r="S37"/>
-      <c r="Y37" s="8" t="s">
+      <c r="Y37" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="Z37" s="14" t="s">
+      <c r="Z37" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="AF37" s="13"/>
-      <c r="AG37" s="12"/>
-      <c r="AH37" s="11"/>
-      <c r="AM37" s="8" t="s">
+      <c r="AF37" s="10"/>
+      <c r="AG37" s="9"/>
+      <c r="AH37" s="8"/>
+      <c r="AM37" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="AN37" s="14" t="s">
+      <c r="AN37" s="11" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="38" spans="15:40" x14ac:dyDescent="0.25">
-      <c r="R38" s="10"/>
+      <c r="R38" s="7"/>
       <c r="S38"/>
-      <c r="AF38" s="13"/>
-      <c r="AG38" s="12"/>
-      <c r="AH38" s="11"/>
+      <c r="AF38" s="10"/>
+      <c r="AG38" s="9"/>
+      <c r="AH38" s="8"/>
     </row>
     <row r="39" spans="15:40" x14ac:dyDescent="0.25">
-      <c r="R39" s="10"/>
+      <c r="R39" s="7"/>
       <c r="S39"/>
-      <c r="AF39" s="13"/>
-      <c r="AG39" s="12"/>
-      <c r="AH39" s="11"/>
+      <c r="AF39" s="10"/>
+      <c r="AG39" s="9"/>
+      <c r="AH39" s="8"/>
     </row>
     <row r="40" spans="15:40" x14ac:dyDescent="0.25">
-      <c r="R40" s="10"/>
+      <c r="R40" s="7"/>
       <c r="S40"/>
-      <c r="Y40" s="20">
+      <c r="Y40" s="17">
         <v>16</v>
       </c>
       <c r="AB40"/>
       <c r="AC40"/>
       <c r="AD40"/>
-      <c r="AF40" s="13"/>
-      <c r="AG40" s="12"/>
-      <c r="AH40" s="11"/>
-      <c r="AM40" s="20">
+      <c r="AF40" s="10"/>
+      <c r="AG40" s="9"/>
+      <c r="AH40" s="8"/>
+      <c r="AM40" s="17">
         <v>9</v>
       </c>
     </row>
     <row r="41" spans="15:40" x14ac:dyDescent="0.25">
-      <c r="R41" s="10"/>
-      <c r="S41" s="10"/>
-      <c r="T41" s="10"/>
-      <c r="U41" s="10"/>
-      <c r="V41" s="10"/>
-      <c r="W41" s="10"/>
-      <c r="X41" s="10"/>
-      <c r="Y41" s="8" t="s">
+      <c r="R41" s="7"/>
+      <c r="S41" s="7"/>
+      <c r="T41" s="7"/>
+      <c r="U41" s="7"/>
+      <c r="V41" s="7"/>
+      <c r="W41" s="7"/>
+      <c r="X41" s="7"/>
+      <c r="Y41" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="Z41" s="9" t="s">
+      <c r="Z41" s="6" t="s">
         <v>53</v>
       </c>
       <c r="AB41"/>
       <c r="AC41"/>
       <c r="AD41"/>
-      <c r="AF41" s="13"/>
-      <c r="AG41" s="12"/>
-      <c r="AH41" s="11"/>
-      <c r="AI41" s="11"/>
-      <c r="AJ41" s="11"/>
-      <c r="AK41" s="11"/>
-      <c r="AL41" s="11"/>
-      <c r="AM41" s="8" t="s">
+      <c r="AF41" s="10"/>
+      <c r="AG41" s="9"/>
+      <c r="AH41" s="8"/>
+      <c r="AI41" s="8"/>
+      <c r="AJ41" s="8"/>
+      <c r="AK41" s="8"/>
+      <c r="AL41" s="8"/>
+      <c r="AM41" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="AN41" s="9" t="s">
+      <c r="AN41" s="6" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="42" spans="15:40" x14ac:dyDescent="0.25">
-      <c r="Y42" s="16" t="s">
+      <c r="Y42" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="Z42" s="5" t="s">
+      <c r="Z42" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="AA42" s="10"/>
-      <c r="AB42" s="5"/>
-      <c r="AC42" s="5"/>
-      <c r="AD42" s="5"/>
-      <c r="AF42" s="13"/>
-      <c r="AG42" s="12"/>
-      <c r="AM42" s="8" t="s">
+      <c r="AA42" s="7"/>
+      <c r="AB42" s="3"/>
+      <c r="AC42" s="3"/>
+      <c r="AD42" s="3"/>
+      <c r="AF42" s="10"/>
+      <c r="AG42" s="9"/>
+      <c r="AM42" s="5" t="s">
         <v>69</v>
       </c>
       <c r="AN42" t="s">
@@ -2394,19 +2370,19 @@
       </c>
     </row>
     <row r="43" spans="15:40" x14ac:dyDescent="0.25">
-      <c r="Y43" s="8" t="s">
+      <c r="Y43" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="Z43" s="4" t="s">
+      <c r="Z43" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="AA43" s="11"/>
-      <c r="AB43" s="4"/>
-      <c r="AC43" s="4"/>
-      <c r="AD43" s="5"/>
-      <c r="AF43" s="13"/>
-      <c r="AG43" s="12"/>
-      <c r="AM43" s="8" t="s">
+      <c r="AA43" s="8"/>
+      <c r="AB43" s="2"/>
+      <c r="AC43" s="2"/>
+      <c r="AD43" s="3"/>
+      <c r="AF43" s="10"/>
+      <c r="AG43" s="9"/>
+      <c r="AM43" s="5" t="s">
         <v>42</v>
       </c>
       <c r="AN43" t="s">
@@ -2414,19 +2390,19 @@
       </c>
     </row>
     <row r="44" spans="15:40" x14ac:dyDescent="0.25">
-      <c r="Y44" s="8" t="s">
+      <c r="Y44" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="Z44" s="15" t="s">
+      <c r="Z44" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="AA44" s="12"/>
-      <c r="AB44" s="15"/>
-      <c r="AC44" s="4"/>
-      <c r="AD44" s="5"/>
-      <c r="AF44" s="13"/>
-      <c r="AG44" s="12"/>
-      <c r="AM44" s="8" t="s">
+      <c r="AA44" s="9"/>
+      <c r="AB44" s="12"/>
+      <c r="AC44" s="2"/>
+      <c r="AD44" s="3"/>
+      <c r="AF44" s="10"/>
+      <c r="AG44" s="9"/>
+      <c r="AM44" s="5" t="s">
         <v>43</v>
       </c>
       <c r="AN44" t="s">
@@ -2434,13 +2410,13 @@
       </c>
     </row>
     <row r="45" spans="15:40" x14ac:dyDescent="0.25">
-      <c r="Y45" s="8"/>
-      <c r="AB45" s="15"/>
-      <c r="AC45" s="4"/>
-      <c r="AD45" s="5"/>
-      <c r="AF45" s="13"/>
-      <c r="AG45" s="12"/>
-      <c r="AM45" s="8" t="s">
+      <c r="Y45" s="5"/>
+      <c r="AB45" s="12"/>
+      <c r="AC45" s="2"/>
+      <c r="AD45" s="3"/>
+      <c r="AF45" s="10"/>
+      <c r="AG45" s="9"/>
+      <c r="AM45" s="5" t="s">
         <v>45</v>
       </c>
       <c r="AN45" t="s">
@@ -2448,72 +2424,72 @@
       </c>
     </row>
     <row r="46" spans="15:40" x14ac:dyDescent="0.25">
-      <c r="Y46" s="8" t="s">
+      <c r="Y46" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="Z46" s="14" t="s">
+      <c r="Z46" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="AB46" s="15"/>
-      <c r="AC46" s="4"/>
-      <c r="AD46" s="5"/>
-      <c r="AF46" s="13"/>
-      <c r="AG46" s="12"/>
-      <c r="AM46" s="8" t="s">
+      <c r="AB46" s="12"/>
+      <c r="AC46" s="2"/>
+      <c r="AD46" s="3"/>
+      <c r="AF46" s="10"/>
+      <c r="AG46" s="9"/>
+      <c r="AM46" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="AN46" s="14" t="s">
+      <c r="AN46" s="11" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="47" spans="15:40" x14ac:dyDescent="0.25">
-      <c r="AB47" s="15"/>
-      <c r="AC47" s="4"/>
-      <c r="AD47" s="5"/>
-      <c r="AF47" s="13"/>
-      <c r="AG47" s="12"/>
+      <c r="AB47" s="12"/>
+      <c r="AC47" s="2"/>
+      <c r="AD47" s="3"/>
+      <c r="AF47" s="10"/>
+      <c r="AG47" s="9"/>
     </row>
     <row r="48" spans="15:40" x14ac:dyDescent="0.25">
-      <c r="AB48" s="15"/>
-      <c r="AC48" s="4"/>
-      <c r="AD48" s="5"/>
-      <c r="AF48" s="13"/>
-      <c r="AG48" s="12"/>
+      <c r="AB48" s="12"/>
+      <c r="AC48" s="2"/>
+      <c r="AD48" s="3"/>
+      <c r="AF48" s="10"/>
+      <c r="AG48" s="9"/>
     </row>
     <row r="49" spans="28:40" x14ac:dyDescent="0.25">
-      <c r="AB49" s="15"/>
-      <c r="AC49" s="4"/>
-      <c r="AD49" s="5"/>
-      <c r="AF49" s="13"/>
-      <c r="AG49" s="12"/>
-      <c r="AM49" s="20">
+      <c r="AB49" s="12"/>
+      <c r="AC49" s="2"/>
+      <c r="AD49" s="3"/>
+      <c r="AF49" s="10"/>
+      <c r="AG49" s="9"/>
+      <c r="AM49" s="17">
         <v>10</v>
       </c>
     </row>
     <row r="50" spans="28:40" x14ac:dyDescent="0.25">
-      <c r="AB50" s="15"/>
-      <c r="AC50" s="4"/>
-      <c r="AD50" s="5"/>
-      <c r="AF50" s="13"/>
-      <c r="AG50" s="12"/>
-      <c r="AH50" s="12"/>
-      <c r="AI50" s="12"/>
-      <c r="AJ50" s="12"/>
-      <c r="AK50" s="12"/>
-      <c r="AL50" s="12"/>
-      <c r="AM50" s="8" t="s">
+      <c r="AB50" s="12"/>
+      <c r="AC50" s="2"/>
+      <c r="AD50" s="3"/>
+      <c r="AF50" s="10"/>
+      <c r="AG50" s="9"/>
+      <c r="AH50" s="9"/>
+      <c r="AI50" s="9"/>
+      <c r="AJ50" s="9"/>
+      <c r="AK50" s="9"/>
+      <c r="AL50" s="9"/>
+      <c r="AM50" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="AN50" s="9" t="s">
+      <c r="AN50" s="6" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="51" spans="28:40" x14ac:dyDescent="0.25">
-      <c r="AB51" s="15"/>
-      <c r="AC51" s="4"/>
-      <c r="AD51" s="5"/>
-      <c r="AF51" s="13"/>
-      <c r="AM51" s="8" t="s">
+      <c r="AB51" s="12"/>
+      <c r="AC51" s="2"/>
+      <c r="AD51" s="3"/>
+      <c r="AF51" s="10"/>
+      <c r="AM51" s="5" t="s">
         <v>44</v>
       </c>
       <c r="AN51" t="s">
@@ -2521,11 +2497,11 @@
       </c>
     </row>
     <row r="52" spans="28:40" x14ac:dyDescent="0.25">
-      <c r="AB52" s="15"/>
-      <c r="AC52" s="4"/>
-      <c r="AD52" s="5"/>
-      <c r="AF52" s="13"/>
-      <c r="AM52" s="8" t="s">
+      <c r="AB52" s="12"/>
+      <c r="AC52" s="2"/>
+      <c r="AD52" s="3"/>
+      <c r="AF52" s="10"/>
+      <c r="AM52" s="5" t="s">
         <v>42</v>
       </c>
       <c r="AN52" t="s">
@@ -2533,11 +2509,11 @@
       </c>
     </row>
     <row r="53" spans="28:40" x14ac:dyDescent="0.25">
-      <c r="AB53" s="15"/>
-      <c r="AC53" s="4"/>
-      <c r="AD53" s="5"/>
-      <c r="AF53" s="13"/>
-      <c r="AM53" s="8" t="s">
+      <c r="AB53" s="12"/>
+      <c r="AC53" s="2"/>
+      <c r="AD53" s="3"/>
+      <c r="AF53" s="10"/>
+      <c r="AM53" s="5" t="s">
         <v>43</v>
       </c>
       <c r="AN53" t="s">
@@ -2545,11 +2521,11 @@
       </c>
     </row>
     <row r="54" spans="28:40" x14ac:dyDescent="0.25">
-      <c r="AB54" s="15"/>
-      <c r="AC54" s="4"/>
-      <c r="AD54" s="5"/>
-      <c r="AF54" s="13"/>
-      <c r="AM54" s="8" t="s">
+      <c r="AB54" s="12"/>
+      <c r="AC54" s="2"/>
+      <c r="AD54" s="3"/>
+      <c r="AF54" s="10"/>
+      <c r="AM54" s="5" t="s">
         <v>74</v>
       </c>
       <c r="AN54" t="s">
@@ -2557,61 +2533,61 @@
       </c>
     </row>
     <row r="55" spans="28:40" x14ac:dyDescent="0.25">
-      <c r="AB55" s="15"/>
-      <c r="AC55" s="4"/>
-      <c r="AD55" s="5"/>
-      <c r="AF55" s="13"/>
-      <c r="AM55" s="8" t="s">
+      <c r="AB55" s="12"/>
+      <c r="AC55" s="2"/>
+      <c r="AD55" s="3"/>
+      <c r="AF55" s="10"/>
+      <c r="AM55" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="AN55" s="14" t="s">
+      <c r="AN55" s="11" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="56" spans="28:40" x14ac:dyDescent="0.25">
-      <c r="AB56" s="15"/>
-      <c r="AC56" s="4"/>
-      <c r="AD56" s="5"/>
-      <c r="AF56" s="13"/>
+      <c r="AB56" s="12"/>
+      <c r="AC56" s="2"/>
+      <c r="AD56" s="3"/>
+      <c r="AF56" s="10"/>
     </row>
     <row r="57" spans="28:40" x14ac:dyDescent="0.25">
-      <c r="AB57" s="15"/>
-      <c r="AC57" s="4"/>
-      <c r="AD57" s="5"/>
-      <c r="AF57" s="13"/>
+      <c r="AB57" s="12"/>
+      <c r="AC57" s="2"/>
+      <c r="AD57" s="3"/>
+      <c r="AF57" s="10"/>
     </row>
     <row r="58" spans="28:40" x14ac:dyDescent="0.25">
-      <c r="AB58" s="15"/>
-      <c r="AC58" s="4"/>
-      <c r="AD58" s="5"/>
-      <c r="AF58" s="13"/>
-      <c r="AM58" s="20">
+      <c r="AB58" s="12"/>
+      <c r="AC58" s="2"/>
+      <c r="AD58" s="3"/>
+      <c r="AF58" s="10"/>
+      <c r="AM58" s="17">
         <v>11</v>
       </c>
     </row>
     <row r="59" spans="28:40" x14ac:dyDescent="0.25">
-      <c r="AB59" s="15"/>
-      <c r="AC59" s="4"/>
-      <c r="AD59" s="5"/>
-      <c r="AF59" s="13"/>
-      <c r="AG59" s="13"/>
-      <c r="AH59" s="13"/>
-      <c r="AI59" s="13"/>
-      <c r="AJ59" s="13"/>
-      <c r="AK59" s="13"/>
-      <c r="AL59" s="13"/>
-      <c r="AM59" s="8" t="s">
+      <c r="AB59" s="12"/>
+      <c r="AC59" s="2"/>
+      <c r="AD59" s="3"/>
+      <c r="AF59" s="10"/>
+      <c r="AG59" s="10"/>
+      <c r="AH59" s="10"/>
+      <c r="AI59" s="10"/>
+      <c r="AJ59" s="10"/>
+      <c r="AK59" s="10"/>
+      <c r="AL59" s="10"/>
+      <c r="AM59" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="AN59" s="9" t="s">
+      <c r="AN59" s="6" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="60" spans="28:40" x14ac:dyDescent="0.25">
-      <c r="AB60" s="15"/>
-      <c r="AC60" s="4"/>
-      <c r="AD60" s="5"/>
-      <c r="AM60" s="8" t="s">
+      <c r="AB60" s="12"/>
+      <c r="AC60" s="2"/>
+      <c r="AD60" s="3"/>
+      <c r="AM60" s="5" t="s">
         <v>44</v>
       </c>
       <c r="AN60" t="s">
@@ -2619,10 +2595,10 @@
       </c>
     </row>
     <row r="61" spans="28:40" x14ac:dyDescent="0.25">
-      <c r="AB61" s="15"/>
-      <c r="AC61" s="4"/>
-      <c r="AD61" s="5"/>
-      <c r="AM61" s="8" t="s">
+      <c r="AB61" s="12"/>
+      <c r="AC61" s="2"/>
+      <c r="AD61" s="3"/>
+      <c r="AM61" s="5" t="s">
         <v>73</v>
       </c>
       <c r="AN61" t="s">
@@ -2630,10 +2606,10 @@
       </c>
     </row>
     <row r="62" spans="28:40" x14ac:dyDescent="0.25">
-      <c r="AB62" s="15"/>
-      <c r="AC62" s="4"/>
-      <c r="AD62" s="5"/>
-      <c r="AM62" s="8" t="s">
+      <c r="AB62" s="12"/>
+      <c r="AC62" s="2"/>
+      <c r="AD62" s="3"/>
+      <c r="AM62" s="5" t="s">
         <v>43</v>
       </c>
       <c r="AN62" t="s">
@@ -2641,10 +2617,10 @@
       </c>
     </row>
     <row r="63" spans="28:40" x14ac:dyDescent="0.25">
-      <c r="AB63" s="15"/>
-      <c r="AC63" s="4"/>
-      <c r="AD63" s="5"/>
-      <c r="AM63" s="8" t="s">
+      <c r="AB63" s="12"/>
+      <c r="AC63" s="2"/>
+      <c r="AD63" s="3"/>
+      <c r="AM63" s="5" t="s">
         <v>45</v>
       </c>
       <c r="AN63" t="s">
@@ -2652,55 +2628,55 @@
       </c>
     </row>
     <row r="64" spans="28:40" x14ac:dyDescent="0.25">
-      <c r="AB64" s="15"/>
-      <c r="AC64" s="4"/>
-      <c r="AD64" s="5"/>
-      <c r="AM64" s="8" t="s">
+      <c r="AB64" s="12"/>
+      <c r="AC64" s="2"/>
+      <c r="AD64" s="3"/>
+      <c r="AM64" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="AN64" s="14" t="s">
+      <c r="AN64" s="11" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="65" spans="28:40" x14ac:dyDescent="0.25">
-      <c r="AB65" s="15"/>
-      <c r="AC65" s="4"/>
-      <c r="AD65" s="5"/>
+      <c r="AB65" s="12"/>
+      <c r="AC65" s="2"/>
+      <c r="AD65" s="3"/>
     </row>
     <row r="66" spans="28:40" x14ac:dyDescent="0.25">
-      <c r="AB66" s="15"/>
-      <c r="AC66" s="4"/>
-      <c r="AD66" s="5"/>
+      <c r="AB66" s="12"/>
+      <c r="AC66" s="2"/>
+      <c r="AD66" s="3"/>
     </row>
     <row r="67" spans="28:40" x14ac:dyDescent="0.25">
-      <c r="AB67" s="15"/>
-      <c r="AC67" s="4"/>
-      <c r="AD67" s="5"/>
-      <c r="AM67" s="20">
+      <c r="AB67" s="12"/>
+      <c r="AC67" s="2"/>
+      <c r="AD67" s="3"/>
+      <c r="AM67" s="17">
         <v>17</v>
       </c>
     </row>
     <row r="68" spans="28:40" x14ac:dyDescent="0.25">
-      <c r="AB68" s="15"/>
-      <c r="AC68" s="4"/>
-      <c r="AD68" s="5"/>
-      <c r="AE68" s="5"/>
-      <c r="AF68" s="5"/>
-      <c r="AG68" s="5"/>
-      <c r="AH68" s="5"/>
-      <c r="AI68" s="5"/>
-      <c r="AJ68" s="5"/>
-      <c r="AK68" s="5"/>
-      <c r="AL68" s="5"/>
-      <c r="AM68" s="8" t="s">
+      <c r="AB68" s="12"/>
+      <c r="AC68" s="2"/>
+      <c r="AD68" s="3"/>
+      <c r="AE68" s="3"/>
+      <c r="AF68" s="3"/>
+      <c r="AG68" s="3"/>
+      <c r="AH68" s="3"/>
+      <c r="AI68" s="3"/>
+      <c r="AJ68" s="3"/>
+      <c r="AK68" s="3"/>
+      <c r="AL68" s="3"/>
+      <c r="AM68" s="5" t="s">
         <v>147</v>
       </c>
       <c r="AN68"/>
     </row>
     <row r="69" spans="28:40" x14ac:dyDescent="0.25">
-      <c r="AB69" s="12"/>
-      <c r="AC69" s="11"/>
-      <c r="AM69" s="16" t="s">
+      <c r="AB69" s="9"/>
+      <c r="AC69" s="8"/>
+      <c r="AM69" s="13" t="s">
         <v>85</v>
       </c>
       <c r="AN69" t="s">
@@ -2708,69 +2684,69 @@
       </c>
     </row>
     <row r="70" spans="28:40" x14ac:dyDescent="0.25">
-      <c r="AB70" s="12"/>
-      <c r="AC70" s="11"/>
-      <c r="AM70" s="8"/>
+      <c r="AB70" s="9"/>
+      <c r="AC70" s="8"/>
+      <c r="AM70" s="5"/>
     </row>
     <row r="71" spans="28:40" x14ac:dyDescent="0.25">
-      <c r="AB71" s="12"/>
-      <c r="AC71" s="11"/>
-      <c r="AM71" s="8" t="s">
+      <c r="AB71" s="9"/>
+      <c r="AC71" s="8"/>
+      <c r="AM71" s="5" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="72" spans="28:40" x14ac:dyDescent="0.25">
-      <c r="AB72" s="12"/>
-      <c r="AC72" s="11"/>
-      <c r="AM72" s="8" t="s">
+      <c r="AB72" s="9"/>
+      <c r="AC72" s="8"/>
+      <c r="AM72" s="5" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="73" spans="28:40" x14ac:dyDescent="0.25">
-      <c r="AB73" s="12"/>
-      <c r="AC73" s="11"/>
-      <c r="AM73" s="8" t="s">
+      <c r="AB73" s="9"/>
+      <c r="AC73" s="8"/>
+      <c r="AM73" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="AN73" s="9" t="s">
+      <c r="AN73" s="6" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="74" spans="28:40" x14ac:dyDescent="0.25">
-      <c r="AB74" s="12"/>
-      <c r="AC74" s="11"/>
+      <c r="AB74" s="9"/>
+      <c r="AC74" s="8"/>
     </row>
     <row r="75" spans="28:40" x14ac:dyDescent="0.25">
-      <c r="AB75" s="12"/>
-      <c r="AC75" s="11"/>
+      <c r="AB75" s="9"/>
+      <c r="AC75" s="8"/>
     </row>
     <row r="76" spans="28:40" x14ac:dyDescent="0.25">
-      <c r="AB76" s="12"/>
-      <c r="AC76" s="11"/>
-      <c r="AM76" s="20">
+      <c r="AB76" s="9"/>
+      <c r="AC76" s="8"/>
+      <c r="AM76" s="17">
         <v>18</v>
       </c>
     </row>
     <row r="77" spans="28:40" x14ac:dyDescent="0.25">
-      <c r="AB77" s="12"/>
-      <c r="AC77" s="11"/>
-      <c r="AD77" s="11"/>
-      <c r="AE77" s="11"/>
-      <c r="AF77" s="11"/>
-      <c r="AG77" s="11"/>
-      <c r="AH77" s="11"/>
-      <c r="AI77" s="11"/>
-      <c r="AJ77" s="11"/>
-      <c r="AK77" s="11"/>
-      <c r="AL77" s="11"/>
-      <c r="AM77" s="8" t="s">
+      <c r="AB77" s="9"/>
+      <c r="AC77" s="8"/>
+      <c r="AD77" s="8"/>
+      <c r="AE77" s="8"/>
+      <c r="AF77" s="8"/>
+      <c r="AG77" s="8"/>
+      <c r="AH77" s="8"/>
+      <c r="AI77" s="8"/>
+      <c r="AJ77" s="8"/>
+      <c r="AK77" s="8"/>
+      <c r="AL77" s="8"/>
+      <c r="AM77" s="5" t="s">
         <v>149</v>
       </c>
       <c r="AN77"/>
     </row>
     <row r="78" spans="28:40" x14ac:dyDescent="0.25">
-      <c r="AB78" s="12"/>
-      <c r="AM78" s="16" t="s">
+      <c r="AB78" s="9"/>
+      <c r="AM78" s="13" t="s">
         <v>83</v>
       </c>
       <c r="AN78" t="s">
@@ -2778,61 +2754,61 @@
       </c>
     </row>
     <row r="79" spans="28:40" x14ac:dyDescent="0.25">
-      <c r="AB79" s="12"/>
-      <c r="AM79" s="8"/>
+      <c r="AB79" s="9"/>
+      <c r="AM79" s="5"/>
     </row>
     <row r="80" spans="28:40" x14ac:dyDescent="0.25">
-      <c r="AB80" s="12"/>
-      <c r="AM80" s="8" t="s">
+      <c r="AB80" s="9"/>
+      <c r="AM80" s="5" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="81" spans="28:40" x14ac:dyDescent="0.25">
-      <c r="AB81" s="12"/>
-      <c r="AM81" s="8" t="s">
+      <c r="AB81" s="9"/>
+      <c r="AM81" s="5" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="82" spans="28:40" x14ac:dyDescent="0.25">
-      <c r="AB82" s="12"/>
-      <c r="AM82" s="8" t="s">
+      <c r="AB82" s="9"/>
+      <c r="AM82" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="AN82" s="9" t="s">
+      <c r="AN82" s="6" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="83" spans="28:40" x14ac:dyDescent="0.25">
-      <c r="AB83" s="12"/>
+      <c r="AB83" s="9"/>
     </row>
     <row r="84" spans="28:40" x14ac:dyDescent="0.25">
-      <c r="AB84" s="12"/>
+      <c r="AB84" s="9"/>
     </row>
     <row r="85" spans="28:40" x14ac:dyDescent="0.25">
-      <c r="AB85" s="12"/>
-      <c r="AM85" s="20">
+      <c r="AB85" s="9"/>
+      <c r="AM85" s="17">
         <v>19</v>
       </c>
     </row>
     <row r="86" spans="28:40" x14ac:dyDescent="0.25">
-      <c r="AB86" s="12"/>
-      <c r="AC86" s="12"/>
-      <c r="AD86" s="12"/>
-      <c r="AE86" s="12"/>
-      <c r="AF86" s="12"/>
-      <c r="AG86" s="12"/>
-      <c r="AH86" s="12"/>
-      <c r="AI86" s="12"/>
-      <c r="AJ86" s="12"/>
-      <c r="AK86" s="12"/>
-      <c r="AL86" s="12"/>
-      <c r="AM86" s="8" t="s">
+      <c r="AB86" s="9"/>
+      <c r="AC86" s="9"/>
+      <c r="AD86" s="9"/>
+      <c r="AE86" s="9"/>
+      <c r="AF86" s="9"/>
+      <c r="AG86" s="9"/>
+      <c r="AH86" s="9"/>
+      <c r="AI86" s="9"/>
+      <c r="AJ86" s="9"/>
+      <c r="AK86" s="9"/>
+      <c r="AL86" s="9"/>
+      <c r="AM86" s="5" t="s">
         <v>148</v>
       </c>
       <c r="AN86"/>
     </row>
     <row r="87" spans="28:40" x14ac:dyDescent="0.25">
-      <c r="AM87" s="16" t="s">
+      <c r="AM87" s="13" t="s">
         <v>84</v>
       </c>
       <c r="AN87" t="s">
@@ -2840,23 +2816,23 @@
       </c>
     </row>
     <row r="88" spans="28:40" x14ac:dyDescent="0.25">
-      <c r="AM88" s="8"/>
+      <c r="AM88" s="5"/>
     </row>
     <row r="89" spans="28:40" x14ac:dyDescent="0.25">
-      <c r="AM89" s="8" t="s">
+      <c r="AM89" s="5" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="90" spans="28:40" x14ac:dyDescent="0.25">
-      <c r="AM90" s="8" t="s">
+      <c r="AM90" s="5" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="91" spans="28:40" x14ac:dyDescent="0.25">
-      <c r="AM91" s="8" t="s">
+      <c r="AM91" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="AN91" s="9" t="s">
+      <c r="AN91" s="6" t="s">
         <v>79</v>
       </c>
     </row>

</xml_diff>

<commit_message>
MENU DRIVEN PROGRAM IS ON FIRE RIGHT NOW
</commit_message>
<xml_diff>
--- a/Arduino/PROTOTYPE4/MENU_DRIVEN_PROGRAM_FLOWCHART.xlsx
+++ b/Arduino/PROTOTYPE4/MENU_DRIVEN_PROGRAM_FLOWCHART.xlsx
@@ -653,6 +653,9 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -661,9 +664,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -993,110 +993,110 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="23"/>
-      <c r="S1" s="23"/>
-      <c r="T1" s="23"/>
-      <c r="U1" s="23"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="M1" s="24"/>
+      <c r="N1" s="24"/>
+      <c r="O1" s="24"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="24"/>
+      <c r="S1" s="24"/>
+      <c r="T1" s="24"/>
+      <c r="U1" s="24"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="24" t="s">
+      <c r="B2" s="24"/>
+      <c r="C2" s="24"/>
+      <c r="D2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="24"/>
-      <c r="H2" s="24"/>
-      <c r="I2" s="24"/>
-      <c r="J2" s="24"/>
-      <c r="K2" s="24"/>
-      <c r="L2" s="24"/>
-      <c r="M2" s="24"/>
-      <c r="N2" s="24"/>
-      <c r="O2" s="24"/>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="24"/>
-      <c r="R2" s="24"/>
-      <c r="S2" s="24"/>
-      <c r="T2" s="24"/>
-      <c r="U2" s="24"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="25"/>
+      <c r="M2" s="25"/>
+      <c r="N2" s="25"/>
+      <c r="O2" s="25"/>
+      <c r="P2" s="25"/>
+      <c r="Q2" s="25"/>
+      <c r="R2" s="25"/>
+      <c r="S2" s="25"/>
+      <c r="T2" s="25"/>
+      <c r="U2" s="25"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="23"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="24" t="s">
+      <c r="E3" s="24"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+      <c r="K3" s="24"/>
+      <c r="L3" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="M3" s="24"/>
-      <c r="N3" s="24"/>
-      <c r="O3" s="24"/>
-      <c r="P3" s="24"/>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="24"/>
-      <c r="S3" s="24"/>
-      <c r="T3" s="24"/>
-      <c r="U3" s="24"/>
+      <c r="M3" s="25"/>
+      <c r="N3" s="25"/>
+      <c r="O3" s="25"/>
+      <c r="P3" s="25"/>
+      <c r="Q3" s="25"/>
+      <c r="R3" s="25"/>
+      <c r="S3" s="25"/>
+      <c r="T3" s="25"/>
+      <c r="U3" s="25"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="E4" s="23"/>
-      <c r="F4" s="23"/>
-      <c r="G4" s="23"/>
-      <c r="H4" s="24"/>
-      <c r="I4" s="24"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="24"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="23"/>
-      <c r="N4" s="24" t="s">
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="25"/>
+      <c r="L4" s="24"/>
+      <c r="M4" s="24"/>
+      <c r="N4" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="O4" s="24"/>
-      <c r="P4" s="24"/>
-      <c r="Q4" s="24"/>
-      <c r="R4" s="24"/>
-      <c r="S4" s="24"/>
-      <c r="T4" s="24"/>
-      <c r="U4" s="24"/>
+      <c r="O4" s="25"/>
+      <c r="P4" s="25"/>
+      <c r="Q4" s="25"/>
+      <c r="R4" s="25"/>
+      <c r="S4" s="25"/>
+      <c r="T4" s="25"/>
+      <c r="U4" s="25"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="23"/>
+      <c r="E5" s="24"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="2"/>
@@ -1105,36 +1105,31 @@
       <c r="K5" s="3"/>
       <c r="L5" s="2"/>
       <c r="M5" s="3"/>
-      <c r="N5" s="23" t="s">
+      <c r="N5" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="O5" s="23"/>
-      <c r="P5" s="23"/>
-      <c r="Q5" s="23"/>
-      <c r="R5" s="24"/>
-      <c r="S5" s="24"/>
-      <c r="T5" s="24"/>
-      <c r="U5" s="24"/>
+      <c r="O5" s="24"/>
+      <c r="P5" s="24"/>
+      <c r="Q5" s="24"/>
+      <c r="R5" s="25"/>
+      <c r="S5" s="25"/>
+      <c r="T5" s="25"/>
+      <c r="U5" s="25"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="N6" s="23" t="s">
+      <c r="N6" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="O6" s="23"/>
-      <c r="P6" s="24"/>
-      <c r="Q6" s="24"/>
-      <c r="R6" s="23"/>
-      <c r="S6" s="23"/>
-      <c r="T6" s="24"/>
-      <c r="U6" s="24"/>
+      <c r="O6" s="24"/>
+      <c r="P6" s="25"/>
+      <c r="Q6" s="25"/>
+      <c r="R6" s="24"/>
+      <c r="S6" s="24"/>
+      <c r="T6" s="25"/>
+      <c r="U6" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A1:U1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="D2:U2"/>
-    <mergeCell ref="D3:K3"/>
-    <mergeCell ref="L3:U3"/>
     <mergeCell ref="N6:O6"/>
     <mergeCell ref="P6:Q6"/>
     <mergeCell ref="R6:S6"/>
@@ -1146,6 +1141,11 @@
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="R5:U5"/>
     <mergeCell ref="N5:Q5"/>
+    <mergeCell ref="A1:U1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="D2:U2"/>
+    <mergeCell ref="D3:K3"/>
+    <mergeCell ref="L3:U3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1155,7 +1155,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AQ91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S40" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I7" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <selection activeCell="AG8" sqref="AG8"/>
     </sheetView>
   </sheetViews>
@@ -1195,7 +1195,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="2:43" s="26" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:43" s="23" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:43" x14ac:dyDescent="0.25">
       <c r="B3" s="15" t="s">
         <v>86</v>
@@ -1276,7 +1276,7 @@
       </c>
       <c r="D5"/>
       <c r="E5"/>
-      <c r="F5" s="25" t="s">
+      <c r="F5" s="26" t="s">
         <v>155</v>
       </c>
       <c r="G5" s="6"/>
@@ -1326,7 +1326,7 @@
       </c>
       <c r="D6"/>
       <c r="E6"/>
-      <c r="F6" s="25"/>
+      <c r="F6" s="26"/>
       <c r="G6" s="7"/>
       <c r="H6" s="5" t="s">
         <v>58</v>
@@ -1364,7 +1364,7 @@
     <row r="7" spans="2:43" x14ac:dyDescent="0.25">
       <c r="D7"/>
       <c r="E7"/>
-      <c r="F7" s="25"/>
+      <c r="F7" s="26"/>
       <c r="G7" s="8"/>
       <c r="H7" s="5" t="s">
         <v>15</v>
@@ -1402,7 +1402,7 @@
     <row r="8" spans="2:43" x14ac:dyDescent="0.25">
       <c r="D8"/>
       <c r="E8"/>
-      <c r="F8" s="25"/>
+      <c r="F8" s="26"/>
       <c r="G8" s="9"/>
       <c r="H8" s="5" t="s">
         <v>100</v>
@@ -1440,7 +1440,7 @@
     <row r="9" spans="2:43" x14ac:dyDescent="0.25">
       <c r="D9"/>
       <c r="E9"/>
-      <c r="F9" s="25"/>
+      <c r="F9" s="26"/>
       <c r="G9" s="10"/>
       <c r="H9" s="5" t="s">
         <v>48</v>
@@ -1468,7 +1468,7 @@
     <row r="10" spans="2:43" x14ac:dyDescent="0.25">
       <c r="D10"/>
       <c r="E10"/>
-      <c r="F10" s="25"/>
+      <c r="F10" s="26"/>
       <c r="G10" s="11"/>
       <c r="H10" s="5" t="s">
         <v>17</v>

</xml_diff>